<commit_message>
added more pictures and refactor code
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AgileConstruction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremynguyen/Documents/GitHub/AgileConstruction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5C3AD2-BC7F-4E0B-8B54-8332C7221436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E80FA0C-3D86-BE44-AD2B-AC2A9D459F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20520" windowHeight="13752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15460" yWindow="6420" windowWidth="20520" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -378,21 +377,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.109375" style="2"/>
+    <col min="2" max="3" width="9.1640625" style="2"/>
     <col min="4" max="4" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44843</v>
       </c>
@@ -411,11 +410,11 @@
         <v>1.5</v>
       </c>
       <c r="D2" s="2">
-        <f>SUM(B2:B100)*30</f>
-        <v>174.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <f>SUM(B2:B100)*45</f>
+        <v>352.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>44844</v>
       </c>
@@ -423,7 +422,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44844</v>
       </c>
@@ -431,12 +430,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44845</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>44930</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>